<commit_message>
removed some useless code, added new albums and their URIs
</commit_message>
<xml_diff>
--- a/backup.xlsx
+++ b/backup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kareem\git\NFC-jukebox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980960CD-C244-48C4-BD04-E5720C72C785}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452B8B8C-1376-4077-9CAF-18A4B179E613}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23430" yWindow="1860" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27495" yWindow="2475" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="backup" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="86">
   <si>
     <t>ID</t>
   </si>
@@ -34,9 +34,6 @@
     <t>URI</t>
   </si>
   <si>
-    <t>Beach Boys</t>
-  </si>
-  <si>
     <t>Smiley Smile</t>
   </si>
   <si>
@@ -71,13 +68,223 @@
   </si>
   <si>
     <t>584198194532</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Beatles </t>
+  </si>
+  <si>
+    <t>Rubber Soul</t>
+  </si>
+  <si>
+    <t>Dark Side Of The Moon</t>
+  </si>
+  <si>
+    <t>Pink Floyd</t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>Bob Marley and The Wailers</t>
+  </si>
+  <si>
+    <t>The Beatles</t>
+  </si>
+  <si>
+    <t>Sgt. Pepper’s Lonely Hearts Club Band</t>
+  </si>
+  <si>
+    <t>What’s Going On</t>
+  </si>
+  <si>
+    <t>Marvin Gaye</t>
+  </si>
+  <si>
+    <t>London Calling</t>
+  </si>
+  <si>
+    <t>The Clash</t>
+  </si>
+  <si>
+    <t>Abbey Road</t>
+  </si>
+  <si>
+    <t>Who’s Next</t>
+  </si>
+  <si>
+    <t>The Who</t>
+  </si>
+  <si>
+    <t>Let It Bleed</t>
+  </si>
+  <si>
+    <t>The Rolling Stones</t>
+  </si>
+  <si>
+    <t>Hotel California</t>
+  </si>
+  <si>
+    <t>The Eagles</t>
+  </si>
+  <si>
+    <t>Please Please Me</t>
+  </si>
+  <si>
+    <t>The Doors</t>
+  </si>
+  <si>
+    <t>A$AP ROCKY</t>
+  </si>
+  <si>
+    <t>AT.LONG.LAST.A$AP</t>
+  </si>
+  <si>
+    <t>Travis Scott</t>
+  </si>
+  <si>
+    <t>Rodeo</t>
+  </si>
+  <si>
+    <t>My Beautiful Dark Twisted Fantasy</t>
+  </si>
+  <si>
+    <t>Kanye West</t>
+  </si>
+  <si>
+    <t>spotify:album:50o7kf2wLwVmOTVYJOTplm</t>
+  </si>
+  <si>
+    <t>spotify:album:4LH4d3cOWNNsVw41Gqt2kv</t>
+  </si>
+  <si>
+    <t>spotify:album:04VRfesff9bgDA2Q8J2oDo</t>
+  </si>
+  <si>
+    <t>spotify:album:6b7ycwe2rxq6FkaupNuGoS</t>
+  </si>
+  <si>
+    <t>spotify:album:6MtwL9RtB8O3s9lJ5RvZHA</t>
+  </si>
+  <si>
+    <t>Surfin' U.S.A</t>
+  </si>
+  <si>
+    <t>The Beach Boys</t>
+  </si>
+  <si>
+    <t>spotify:album:6qX4eoPWGteMdJMqGOwPTs</t>
+  </si>
+  <si>
+    <t>spotify:album:6FCzvataOZh68j8OKzOt9a</t>
+  </si>
+  <si>
+    <t>spotify:album:5iT3F2EhjVQVrO4PKhsP8c</t>
+  </si>
+  <si>
+    <t>spotify:album:5MqyhhHbT13zsloD3uHhlQ</t>
+  </si>
+  <si>
+    <t>spotify:album:4l4u9e9jSbotSXNjYfOugy</t>
+  </si>
+  <si>
+    <t>spotify:album:2widuo17g5CEC66IbzveRu</t>
+  </si>
+  <si>
+    <t>spotify:album:3KzAvEXcqJKBF97HrXwlgf</t>
+  </si>
+  <si>
+    <t>spotify:album:1jWmEhn3ggaL6isoyLfwBn</t>
+  </si>
+  <si>
+    <t>L.A. Woman</t>
+  </si>
+  <si>
+    <t>spotify:album:7IKUTIc9UWuVngyGPtqNHS</t>
+  </si>
+  <si>
+    <t>spotify:album:3arNdjotCvtiiLFfjKngMc</t>
+  </si>
+  <si>
+    <t>spotify:album:4PWBTB6NYSKQwfo79I3prg</t>
+  </si>
+  <si>
+    <t>spotify:album:20r762YmB5HeofjMCiPMLv</t>
+  </si>
+  <si>
+    <t>spotify:album:4xwx0x7k6c5VuThz5qVqmV</t>
+  </si>
+  <si>
+    <t>The Velvet Underground, Nico</t>
+  </si>
+  <si>
+    <t>The Velvet Underground and Nico</t>
+  </si>
+  <si>
+    <t>Born In The USA</t>
+  </si>
+  <si>
+    <t>Bruce Springsteen</t>
+  </si>
+  <si>
+    <t>spotify:album:0PMasrHdpaoIRuHuhHp72O</t>
+  </si>
+  <si>
+    <t>Cake</t>
+  </si>
+  <si>
+    <t>Comfort Eagle</t>
+  </si>
+  <si>
+    <t>spotify:album:5OCg9OWnL1PY4tW2ON8ssj</t>
+  </si>
+  <si>
+    <t>spotify:album:11oR0ZuqB3ucZwb5TGbZxb</t>
+  </si>
+  <si>
+    <t>Beastie Boys</t>
+  </si>
+  <si>
+    <t>License to III</t>
+  </si>
+  <si>
+    <t>Guns N' Roses</t>
+  </si>
+  <si>
+    <t>Use Your Illusion II</t>
+  </si>
+  <si>
+    <t>spotify:album:5mzoB7ggIOyQIzj5sGl0ZH</t>
+  </si>
+  <si>
+    <t>Spirit Of America</t>
+  </si>
+  <si>
+    <t>spotify:album:1reJ8DttK5EGwdyf7y9FBR</t>
+  </si>
+  <si>
+    <t>Elton John</t>
+  </si>
+  <si>
+    <t>Don't Shoot Me I'm Only The Piano Player</t>
+  </si>
+  <si>
+    <t>spotify:album:1j3ak8bXvTij3YcWXb6laH</t>
+  </si>
+  <si>
+    <t>PLAYLIST</t>
+  </si>
+  <si>
+    <t>spotify:playlist:5NedNTv3hA6ZwoLSRAiDsa</t>
+  </si>
+  <si>
+    <t>NFC Party List</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,6 +415,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -554,12 +769,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -915,49 +1131,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" customWidth="1"/>
-    <col min="4" max="4" width="37.28515625" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="38" customWidth="1"/>
+    <col min="4" max="4" width="45.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>13</v>
+      <c r="E1" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -965,16 +1181,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -982,16 +1198,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2">
         <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -999,7 +1215,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -1007,40 +1232,456 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
       </c>
       <c r="E6">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
       <c r="E7">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
       <c r="E8">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
       <c r="E9">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
       <c r="E10">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>51</v>
+      </c>
       <c r="E11">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>52</v>
+      </c>
       <c r="E12">
         <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" t="s">
+        <v>82</v>
+      </c>
+      <c r="E27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added up to 61 new albums
</commit_message>
<xml_diff>
--- a/backup.xlsx
+++ b/backup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kareem\git\NFC-jukebox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452B8B8C-1376-4077-9CAF-18A4B179E613}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E8B7DFF-8155-4437-98D8-D9B61D6C3129}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27495" yWindow="2475" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="backup" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="173">
   <si>
     <t>ID</t>
   </si>
@@ -278,6 +278,267 @@
   </si>
   <si>
     <t>NFC Party List</t>
+  </si>
+  <si>
+    <t>spotify:album:6trNtQUgC8cgbWcqoMYkOR</t>
+  </si>
+  <si>
+    <t>Post Malone</t>
+  </si>
+  <si>
+    <t>beerbongs &amp; bentleys</t>
+  </si>
+  <si>
+    <t>Various Artists</t>
+  </si>
+  <si>
+    <t>Another Shot of Old Skool of Rock</t>
+  </si>
+  <si>
+    <t>spotify:album:3UioHiThwqh7dbae38V3Ib</t>
+  </si>
+  <si>
+    <t>Appetite For Destruction</t>
+  </si>
+  <si>
+    <t>spotify:album:28yHV3Gdg30AiB8h8em1eW</t>
+  </si>
+  <si>
+    <t>Watch The Throne</t>
+  </si>
+  <si>
+    <t>JAY-Z, Kanye West</t>
+  </si>
+  <si>
+    <t>spotify:album:2P2Xwvh2xWXIZ1OWY9S9o5</t>
+  </si>
+  <si>
+    <t>Dr. Dre</t>
+  </si>
+  <si>
+    <t>spotify:album:7q2B4M5EiBkqrlsNW8lB7N</t>
+  </si>
+  <si>
+    <t>Graduation</t>
+  </si>
+  <si>
+    <t>spotify:album:5fPglEDz9YEwRgbLRvhCZy</t>
+  </si>
+  <si>
+    <t>12 Sa'a</t>
+  </si>
+  <si>
+    <t>Adonis</t>
+  </si>
+  <si>
+    <t>spotify:album:7yWLsrNU17dhFesO9R7EZa</t>
+  </si>
+  <si>
+    <t>Freeze Frame</t>
+  </si>
+  <si>
+    <t>spotify:album:48joW5905AMbTFLvy8ZWch</t>
+  </si>
+  <si>
+    <t>The J. Geils Band</t>
+  </si>
+  <si>
+    <t>AC/DC</t>
+  </si>
+  <si>
+    <t>Back In Black</t>
+  </si>
+  <si>
+    <t>spotify:album:6mUdeDZCsExyJLMdAfDuwh</t>
+  </si>
+  <si>
+    <t>spotify:album:4vu7F6h90Br1ZtYYaqfITy</t>
+  </si>
+  <si>
+    <t>The Razor's Edge</t>
+  </si>
+  <si>
+    <t>Highway To Hell</t>
+  </si>
+  <si>
+    <t>spotify:album:10v912xgTZbjAtYfyKWJCS</t>
+  </si>
+  <si>
+    <t>spotify:album:4wExFfncaUIqSgoxnqa3Eh</t>
+  </si>
+  <si>
+    <t>Led Zeppelin</t>
+  </si>
+  <si>
+    <t>Mothership</t>
+  </si>
+  <si>
+    <t>spotify:album:4teFaDSeFHYXZjZJaZGrAO</t>
+  </si>
+  <si>
+    <t>The White Stripes</t>
+  </si>
+  <si>
+    <t>Elephant</t>
+  </si>
+  <si>
+    <t>Oasis</t>
+  </si>
+  <si>
+    <t>Definitely Maybe</t>
+  </si>
+  <si>
+    <t>spotify:album:6YS4zNofCOD5Kf9H39WHNI</t>
+  </si>
+  <si>
+    <t>spotify:album:29m6DinzdaD0OPqWKGyMdz</t>
+  </si>
+  <si>
+    <t>Sticky Fingers</t>
+  </si>
+  <si>
+    <t>Exile on Main St.</t>
+  </si>
+  <si>
+    <t>spotify:album:5U4dnRZsfW8NmwBBkELFPh</t>
+  </si>
+  <si>
+    <t>Paul's Boutique</t>
+  </si>
+  <si>
+    <t>spotify:album:1kmyirVya5fRxdjsPFDM05</t>
+  </si>
+  <si>
+    <t>Nirvana</t>
+  </si>
+  <si>
+    <t>Nevermind</t>
+  </si>
+  <si>
+    <t>spotify:album:6yaiubHHJy8N8QcHy3julo</t>
+  </si>
+  <si>
+    <t>Pearl Jam</t>
+  </si>
+  <si>
+    <t>spotify:album:5B4PYA7wNN4WdEXdIJu58a</t>
+  </si>
+  <si>
+    <t>Ten</t>
+  </si>
+  <si>
+    <t>spotify:album:7dxKtc08dYeRVHt3p9CZJn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radiohead </t>
+  </si>
+  <si>
+    <t>OK Computer</t>
+  </si>
+  <si>
+    <t>David Bowie</t>
+  </si>
+  <si>
+    <t>spotify:album:48D1hRORqJq52qsnUYZX56</t>
+  </si>
+  <si>
+    <t>spotify:album:4I5zzKYd2SKDgZ9DRf5LVk</t>
+  </si>
+  <si>
+    <t>Heroes</t>
+  </si>
+  <si>
+    <t>Pet Sounds</t>
+  </si>
+  <si>
+    <t>Greetings from Asbury Park</t>
+  </si>
+  <si>
+    <t>spotify:album:4hQ5RfHzq1SGJNfZWrpg7C</t>
+  </si>
+  <si>
+    <t>spotify:album:42oBdomfxF0DbKKMEqrnQW</t>
+  </si>
+  <si>
+    <t>Rumours</t>
+  </si>
+  <si>
+    <t>Fleetwood Mac</t>
+  </si>
+  <si>
+    <t>spotify:album:1bt6q2SruMsBtcerNVtpZB</t>
+  </si>
+  <si>
+    <t>Prince</t>
+  </si>
+  <si>
+    <t>spotify:album:7nXJ5k4XgRj5OLg9m8V3zc</t>
+  </si>
+  <si>
+    <t>Purple Rain</t>
+  </si>
+  <si>
+    <t>spotify:album:3PRoXYsngSwjEQWR5PsHWR</t>
+  </si>
+  <si>
+    <t>Revolver</t>
+  </si>
+  <si>
+    <t>NWA</t>
+  </si>
+  <si>
+    <t>spotify:album:0Y7qkJVZ06tS2GUCDptzyW</t>
+  </si>
+  <si>
+    <t>Straight Outta Compton</t>
+  </si>
+  <si>
+    <t>JAY-Z</t>
+  </si>
+  <si>
+    <t>spotify:album:2CUT0104gySOIvqwtXeFsX</t>
+  </si>
+  <si>
+    <t>Kendrick Lamar</t>
+  </si>
+  <si>
+    <t>good kid, m.A.A.d. city</t>
+  </si>
+  <si>
+    <t>spotify:album:3DGQ1iZ9XKUQxAUWjfC34w</t>
+  </si>
+  <si>
+    <t>spotify:album:78bpIziExqiI9qztvNFlQu</t>
+  </si>
+  <si>
+    <t>Arctic Monkeys</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>The Rise and Fall of Ziggy Stardust and the Spiders from Mars</t>
+  </si>
+  <si>
+    <t>The Blueprint III</t>
+  </si>
+  <si>
+    <t>spotify:album:1woCvthHJakakroP6dXNxs</t>
+  </si>
+  <si>
+    <t>Wicked</t>
+  </si>
+  <si>
+    <t>Hamilton</t>
+  </si>
+  <si>
+    <t>spotify:album:1kCHru7uhxBUdzkm4gzRQc</t>
+  </si>
+  <si>
+    <t>spotify:album:6QtnCAFmqOwR75jOOmU7k9</t>
+  </si>
+  <si>
+    <t>Mamma Mia!</t>
   </si>
 </sst>
 </file>
@@ -428,7 +689,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -606,6 +867,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -769,13 +1036,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1131,17 +1400,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.85546875" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
-    <col min="3" max="3" width="38" customWidth="1"/>
+    <col min="3" max="3" width="61.7109375" customWidth="1"/>
     <col min="4" max="4" width="45.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1570,121 +1839,501 @@
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" t="s">
+        <v>86</v>
+      </c>
       <c r="E30">
         <v>28</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" t="s">
+        <v>91</v>
+      </c>
       <c r="E31">
         <v>29</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" t="s">
+        <v>93</v>
+      </c>
       <c r="E32">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D33" t="s">
+        <v>96</v>
+      </c>
       <c r="E33">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="2">
+        <v>2001</v>
+      </c>
+      <c r="D34" t="s">
+        <v>98</v>
+      </c>
       <c r="E34">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" t="s">
+        <v>100</v>
+      </c>
       <c r="E35">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" t="s">
+        <v>101</v>
+      </c>
+      <c r="D36" t="s">
+        <v>103</v>
+      </c>
       <c r="E36">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>106</v>
+      </c>
+      <c r="C37" t="s">
+        <v>104</v>
+      </c>
+      <c r="D37" t="s">
+        <v>105</v>
+      </c>
       <c r="E37">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38" t="s">
+        <v>108</v>
+      </c>
+      <c r="D38" t="s">
+        <v>109</v>
+      </c>
       <c r="E38">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" t="s">
+        <v>107</v>
+      </c>
+      <c r="C39" t="s">
+        <v>111</v>
+      </c>
+      <c r="D39" t="s">
+        <v>110</v>
+      </c>
       <c r="E39">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" t="s">
+        <v>112</v>
+      </c>
+      <c r="D40" t="s">
+        <v>113</v>
+      </c>
       <c r="E40">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" t="s">
+        <v>115</v>
+      </c>
+      <c r="C41" t="s">
+        <v>116</v>
+      </c>
+      <c r="D41" t="s">
+        <v>114</v>
+      </c>
       <c r="E41">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" t="s">
+        <v>118</v>
+      </c>
+      <c r="C42" t="s">
+        <v>119</v>
+      </c>
+      <c r="D42" t="s">
+        <v>117</v>
+      </c>
       <c r="E42">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43" t="s">
+        <v>121</v>
+      </c>
+      <c r="D43" t="s">
+        <v>122</v>
+      </c>
       <c r="E43">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D44" t="s">
+        <v>123</v>
+      </c>
       <c r="E44">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" t="s">
+        <v>32</v>
+      </c>
+      <c r="C45" t="s">
+        <v>125</v>
+      </c>
+      <c r="D45" t="s">
+        <v>126</v>
+      </c>
       <c r="E45">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" t="s">
+        <v>73</v>
+      </c>
+      <c r="C46" t="s">
+        <v>127</v>
+      </c>
+      <c r="D46" t="s">
+        <v>128</v>
+      </c>
       <c r="E46">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" t="s">
+        <v>129</v>
+      </c>
+      <c r="C47" t="s">
+        <v>130</v>
+      </c>
+      <c r="D47" t="s">
+        <v>131</v>
+      </c>
       <c r="E47">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" t="s">
+        <v>132</v>
+      </c>
+      <c r="C48" t="s">
+        <v>134</v>
+      </c>
+      <c r="D48" t="s">
+        <v>133</v>
+      </c>
       <c r="E48">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" t="s">
+        <v>136</v>
+      </c>
+      <c r="C49" t="s">
+        <v>137</v>
+      </c>
+      <c r="D49" t="s">
+        <v>135</v>
+      </c>
       <c r="E49">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" t="s">
+        <v>138</v>
+      </c>
+      <c r="C50" t="s">
+        <v>165</v>
+      </c>
+      <c r="D50" t="s">
+        <v>139</v>
+      </c>
       <c r="E50">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+      <c r="B51" t="s">
+        <v>138</v>
+      </c>
+      <c r="C51" t="s">
+        <v>141</v>
+      </c>
+      <c r="D51" t="s">
+        <v>140</v>
+      </c>
       <c r="E51">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" t="s">
+        <v>49</v>
+      </c>
+      <c r="C52" t="s">
+        <v>142</v>
+      </c>
+      <c r="D52" t="s">
+        <v>145</v>
+      </c>
       <c r="E52">
         <v>50</v>
       </c>
     </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>67</v>
+      </c>
+      <c r="C53" t="s">
+        <v>143</v>
+      </c>
+      <c r="D53" t="s">
+        <v>144</v>
+      </c>
+      <c r="E53">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>147</v>
+      </c>
+      <c r="C54" t="s">
+        <v>146</v>
+      </c>
+      <c r="D54" t="s">
+        <v>148</v>
+      </c>
+      <c r="E54">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>149</v>
+      </c>
+      <c r="C55" t="s">
+        <v>151</v>
+      </c>
+      <c r="D55" t="s">
+        <v>150</v>
+      </c>
+      <c r="E55">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>22</v>
+      </c>
+      <c r="C56" t="s">
+        <v>153</v>
+      </c>
+      <c r="D56" t="s">
+        <v>152</v>
+      </c>
+      <c r="E56">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>154</v>
+      </c>
+      <c r="C57" t="s">
+        <v>156</v>
+      </c>
+      <c r="D57" t="s">
+        <v>155</v>
+      </c>
+      <c r="E57">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>157</v>
+      </c>
+      <c r="C58" t="s">
+        <v>166</v>
+      </c>
+      <c r="D58" t="s">
+        <v>158</v>
+      </c>
+      <c r="E58">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>159</v>
+      </c>
+      <c r="C59" t="s">
+        <v>160</v>
+      </c>
+      <c r="D59" t="s">
+        <v>161</v>
+      </c>
+      <c r="E59">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>163</v>
+      </c>
+      <c r="C60" t="s">
+        <v>164</v>
+      </c>
+      <c r="D60" t="s">
+        <v>162</v>
+      </c>
+      <c r="E60">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="5"/>
+      <c r="B61" t="s">
+        <v>89</v>
+      </c>
+      <c r="C61" t="s">
+        <v>168</v>
+      </c>
+      <c r="D61" t="s">
+        <v>167</v>
+      </c>
+      <c r="E61">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>89</v>
+      </c>
+      <c r="C62" t="s">
+        <v>169</v>
+      </c>
+      <c r="D62" t="s">
+        <v>170</v>
+      </c>
+      <c r="E62">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>89</v>
+      </c>
+      <c r="C63" t="s">
+        <v>172</v>
+      </c>
+      <c r="D63" t="s">
+        <v>171</v>
+      </c>
+      <c r="E63">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:D4">
+    <sortCondition ref="B4"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>